<commit_message>
PROS-6529 - BITH Template update
</commit_message>
<xml_diff>
--- a/Projects/BITH/Data/Template.xlsx
+++ b/Projects/BITH/Data/Template.xlsx
@@ -1465,13 +1465,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.6356275303644"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1735,12 +1735,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2094,11 +2094,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="26" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="31.0647773279352"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="26" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="1023" min="7" style="14" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.89068825910931"/>
   </cols>
@@ -2112,6 +2112,7 @@
       <c r="F1" s="16" t="s">
         <v>30</v>
       </c>
+      <c r="G1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
@@ -2304,9 +2305,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="43.17004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="43.5991902834008"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="38.8825910931174"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="34" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="35" width="8.89068825910931"/>
   </cols>
@@ -2456,12 +2457,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="42" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="42" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="42" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="42" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="42" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="42" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="43" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2677,17 +2678,17 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="55" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="55" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="55" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="55" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="55" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="55" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="55" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="55" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="55" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="55" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="55" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="56" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2758,7 +2759,7 @@
         <v>38</v>
       </c>
       <c r="F4" s="60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-7064 BATAU - Simon and KPIs Change to include Zero %
</commit_message>
<xml_diff>
--- a/Projects/BITH/Data/Template.xlsx
+++ b/Projects/BITH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -1488,13 +1488,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.2793522267206"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1752,18 +1752,18 @@
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.0242914979757"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2005,7 +2005,7 @@
         <v>52</v>
       </c>
       <c r="F12" s="24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="0"/>
     </row>
@@ -2047,7 +2047,7 @@
         <v>38</v>
       </c>
       <c r="F14" s="24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="25"/>
     </row>
@@ -2089,7 +2089,7 @@
         <v>46</v>
       </c>
       <c r="F16" s="24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2117,11 +2117,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="26" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="26" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="1023" min="7" style="14" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.89068825910931"/>
   </cols>
@@ -2322,15 +2322,15 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="43.919028340081"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="44.2388663967611"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="39.5263157894737"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="34" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="35" width="8.89068825910931"/>
   </cols>
@@ -2471,12 +2471,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="32.7773279352227"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="46" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="46" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="46" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="46" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="47" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2697,12 +2697,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="59" width="31.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="59" width="43.7044534412956"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="59" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="59" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="59" width="44.0242914979757"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="59" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="59" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="59" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="59" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="60" width="8.89068825910931"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
PROS-7071 - BITH - Monthly Template changes
</commit_message>
<xml_diff>
--- a/Projects/BITH/Data/Template.xlsx
+++ b/Projects/BITH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -538,7 +538,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="80">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -1137,7 +1137,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1312,14 +1312,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1488,13 +1480,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1752,18 +1744,18 @@
   </sheetPr>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.0242914979757"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2117,11 +2109,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="26" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="31.8137651821862"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="26" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="1023" min="7" style="14" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.89068825910931"/>
   </cols>
@@ -2322,15 +2314,15 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="44.2388663967611"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="39.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="44.5627530364373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="39.8502024291498"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="34" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="35" width="8.89068825910931"/>
   </cols>
@@ -2425,26 +2417,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2471,13 +2445,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="46" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="46" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="47" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="45" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2491,30 +2465,30 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="47" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="49" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="25" t="s">
@@ -2523,18 +2497,18 @@
       <c r="D3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="53" t="n">
+      <c r="F3" s="51" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="49" t="s">
         <v>71</v>
       </c>
       <c r="C4" s="25" t="s">
@@ -2546,15 +2520,15 @@
       <c r="E4" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="53" t="n">
+      <c r="F4" s="51" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="49" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="25" t="s">
@@ -2563,18 +2537,18 @@
       <c r="D5" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="54" t="n">
+      <c r="F5" s="52" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="54" t="s">
         <v>75</v>
       </c>
       <c r="C6" s="25" t="s">
@@ -2583,42 +2557,42 @@
       <c r="D6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="57" t="n">
+      <c r="F6" s="55" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="53" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
-      <c r="F7" s="53"/>
+      <c r="F7" s="51"/>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
-      <c r="E8" s="58"/>
+      <c r="E8" s="56"/>
       <c r="F8" s="30"/>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
-      <c r="E9" s="58"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="30"/>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
-      <c r="E10" s="58"/>
+      <c r="E10" s="56"/>
       <c r="F10" s="30"/>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2697,13 +2671,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="59" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="59" width="44.0242914979757"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="59" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="59" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="59" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="60" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="57" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="57" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="57" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="57" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="57" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="57" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="58" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2717,33 +2691,33 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="59" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="60" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="63" t="n">
+      <c r="C3" s="61" t="n">
         <v>8850886103072</v>
       </c>
       <c r="D3" s="20" t="s">
@@ -2752,18 +2726,18 @@
       <c r="E3" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="64" t="n">
+      <c r="F3" s="62" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="60" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="63" t="n">
+      <c r="C4" s="61" t="n">
         <v>8850886103041</v>
       </c>
       <c r="D4" s="20" t="s">
@@ -2772,18 +2746,18 @@
       <c r="E4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="64" t="n">
+      <c r="F4" s="62" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="60" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="63" t="n">
+      <c r="C5" s="61" t="n">
         <v>8850886103058</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -2792,18 +2766,18 @@
       <c r="E5" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="64" t="n">
+      <c r="F5" s="62" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="60" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="63" t="n">
+      <c r="C6" s="61" t="n">
         <v>8850886103126</v>
       </c>
       <c r="D6" s="20" t="s">
@@ -2812,18 +2786,18 @@
       <c r="E6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="64" t="n">
+      <c r="F6" s="62" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="60" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="63" t="n">
+      <c r="C7" s="61" t="n">
         <v>8850886103133</v>
       </c>
       <c r="D7" s="20" t="s">
@@ -2832,18 +2806,18 @@
       <c r="E7" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="64" t="n">
+      <c r="F7" s="62" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="60" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="63" t="n">
+      <c r="C8" s="61" t="n">
         <v>8993237285017</v>
       </c>
       <c r="D8" s="20" t="s">
@@ -2852,18 +2826,18 @@
       <c r="E8" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="64" t="n">
+      <c r="F8" s="62" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="60" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="63" t="n">
+      <c r="C9" s="61" t="n">
         <v>8993237226072</v>
       </c>
       <c r="D9" s="20" t="s">
@@ -2872,18 +2846,18 @@
       <c r="E9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="64" t="n">
+      <c r="F9" s="62" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="60" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="63" t="n">
+      <c r="C10" s="61" t="n">
         <v>7891058013264</v>
       </c>
       <c r="D10" s="20" t="s">
@@ -2892,18 +2866,18 @@
       <c r="E10" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="64" t="n">
+      <c r="F10" s="62" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="63" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="63" t="n">
+      <c r="C11" s="61" t="n">
         <v>8850886103072</v>
       </c>
       <c r="D11" s="20" t="s">
@@ -2912,18 +2886,18 @@
       <c r="E11" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="64" t="n">
+      <c r="F11" s="62" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="63" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="63" t="n">
+      <c r="C12" s="61" t="n">
         <v>8850886103041</v>
       </c>
       <c r="D12" s="20" t="s">
@@ -2932,18 +2906,18 @@
       <c r="E12" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="64" t="n">
+      <c r="F12" s="62" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="63" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="63" t="n">
+      <c r="C13" s="61" t="n">
         <v>8850886103058</v>
       </c>
       <c r="D13" s="20" t="s">
@@ -2952,18 +2926,18 @@
       <c r="E13" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="64" t="n">
+      <c r="F13" s="62" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="63" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="63" t="n">
+      <c r="C14" s="61" t="n">
         <v>8850886057252</v>
       </c>
       <c r="D14" s="20" t="s">
@@ -2972,18 +2946,18 @@
       <c r="E14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="64" t="n">
+      <c r="F14" s="62" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="63" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="63" t="n">
+      <c r="C15" s="61" t="n">
         <v>8850886057207</v>
       </c>
       <c r="D15" s="20" t="s">
@@ -2992,7 +2966,7 @@
       <c r="E15" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="64" t="n">
+      <c r="F15" s="62" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROS-7525 BITH Kpi Update
</commit_message>
<xml_diff>
--- a/Projects/BITH/Data/Template.xlsx
+++ b/Projects/BITH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -538,7 +538,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="68">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -702,30 +702,18 @@
     <t xml:space="preserve">Telfast 180 MG</t>
   </si>
   <si>
-    <t xml:space="preserve">Telfast Oral Suspension 150ml</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maalox Alum Milk 240ml</t>
   </si>
   <si>
     <t xml:space="preserve">Maalox</t>
   </si>
   <si>
-    <t xml:space="preserve">Mucosolvan Syrup 60ml</t>
+    <t xml:space="preserve">Mucosolvan Tab 30mg</t>
   </si>
   <si>
     <t xml:space="preserve">Mucosolvan</t>
   </si>
   <si>
-    <t xml:space="preserve">Mucosolvan Tab 30mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proctosedyl Oint 15mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proctosedyl</t>
-  </si>
-  <si>
     <t xml:space="preserve">SKUs</t>
   </si>
   <si>
@@ -751,12 +739,6 @@
   </si>
   <si>
     <t xml:space="preserve">TH_Secondary_04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bisolvon Tab 8 MG 50x10's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUCOSOLVAN SYRUB 60ml</t>
   </si>
   <si>
     <t xml:space="preserve">MUCOSOLVAN TAB 30mg</t>
@@ -1419,19 +1401,19 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1687,20 +1669,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -1933,102 +1915,43 @@
         <v>54</v>
       </c>
       <c r="C12" s="21" t="n">
-        <v>7891058013264</v>
+        <v>8850886056125</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="0"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C13" s="21" t="n">
-        <v>8850886056125</v>
+        <v>8850886103133</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>46</v>
+        <v>57</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="F13" s="24" t="n">
         <v>1</v>
       </c>
       <c r="G13" s="25"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="21" t="n">
-        <v>8850886103126</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="25"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="21" t="n">
-        <v>8850886103133</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="25"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="21" t="n">
-        <v>8850886087228</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="24" t="n">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2054,11 +1977,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="26" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="32.2429149797571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="26" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="17.8906882591093"/>
     <col collapsed="false" hidden="false" max="1023" min="7" style="14" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.89068825910931"/>
   </cols>
@@ -2085,7 +2008,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>32</v>
@@ -2259,15 +2182,15 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="44.8825910931174"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="45.2024291497976"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="40.5991902834008"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="34" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="35" width="8.89068825910931"/>
   </cols>
@@ -2327,12 +2250,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="33.5263157894737"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="38" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2371,10 +2294,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>37</v>
@@ -2391,10 +2314,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>51</v>
@@ -2411,13 +2334,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="43" t="s">
         <v>38</v>
@@ -2431,10 +2354,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>37</v>
@@ -2545,20 +2468,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="32.4574898785425"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="44.668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="44.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="50" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="51" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2597,10 +2520,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="C3" s="54" t="n">
-        <v>8850886103072</v>
+        <v>8850886103041</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>37</v>
@@ -2609,7 +2532,7 @@
         <v>38</v>
       </c>
       <c r="F3" s="55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2617,10 +2540,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="54" t="n">
-        <v>8850886103041</v>
+        <v>8850886103058</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>37</v>
@@ -2637,13 +2560,13 @@
         <v>12</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="C5" s="54" t="n">
-        <v>8850886103058</v>
+        <v>8850886103133</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>38</v>
@@ -2657,19 +2580,19 @@
         <v>12</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="C6" s="54" t="n">
-        <v>8850886103126</v>
+        <v>8993237285017</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F6" s="55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,181 +2600,67 @@
         <v>12</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C7" s="54" t="n">
-        <v>8850886103133</v>
+        <v>8993237226072</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F7" s="55" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="53" t="s">
-        <v>12</v>
+      <c r="A8" s="56" t="s">
+        <v>22</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C8" s="54" t="n">
-        <v>8993237285017</v>
+        <v>8850886103058</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>52</v>
+        <v>37</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="F8" s="55" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="53" t="s">
-        <v>12</v>
+      <c r="A9" s="56" t="s">
+        <v>22</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C9" s="54" t="n">
-        <v>8993237226072</v>
+        <v>8850886057252</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="F9" s="55" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="54" t="n">
-        <v>7891058013264</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="55" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="54" t="n">
-        <v>8850886103072</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="55" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="54" t="n">
-        <v>8850886103041</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="55" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="54" t="n">
-        <v>8850886103058</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="55" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="54" t="n">
-        <v>8850886057252</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="55" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="54" t="n">
-        <v>8850886057207</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="55" t="n">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
BITH Template Change - adjusted the MSL updates as per the file attached in PROS-8102
</commit_message>
<xml_diff>
--- a/Projects/BITH/Data/Template.xlsx
+++ b/Projects/BITH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -538,7 +538,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="75">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -712,6 +712,27 @@
   </si>
   <si>
     <t xml:space="preserve">Mucosolvan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bisolvon 8mg syrup 60ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cough&amp;Cold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dulcolax Tablet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dulcolax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pharmaton Cap 30mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pharmaton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutritional</t>
   </si>
   <si>
     <t xml:space="preserve">SKUs</t>
@@ -1193,24 +1214,24 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1407,13 +1428,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1669,20 +1690,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G65536"/>
+  <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -1697,7 +1718,7 @@
       </c>
       <c r="G1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
@@ -1717,6 +1738,7 @@
         <v>35</v>
       </c>
       <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
@@ -1738,6 +1760,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
@@ -1759,6 +1782,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
@@ -1780,6 +1804,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
@@ -1801,6 +1826,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
@@ -1822,6 +1848,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
@@ -1843,6 +1870,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
@@ -1864,6 +1892,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
@@ -1885,6 +1914,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="0"/>
+      <c r="H10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
@@ -1906,6 +1936,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="0"/>
+      <c r="H11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="19" t="s">
@@ -1926,7 +1957,8 @@
       <c r="F12" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="G12" s="25"/>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
@@ -1947,7 +1979,74 @@
       <c r="F13" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="G13" s="25"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="21" t="n">
+        <v>8850886103218</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="21" t="n">
+        <v>4048846004130</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="0"/>
+      <c r="H15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="21" t="n">
+        <v>8850886103171</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="0"/>
+      <c r="H16" s="0"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1977,21 +2076,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="26" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="32.4574898785425"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="26" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="25" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="25" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="25" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="25" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="1023" min="7" style="14" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="16" t="s">
         <v>30</v>
       </c>
@@ -2008,7 +2107,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>32</v>
@@ -2016,20 +2115,20 @@
       <c r="F2" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="28"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
       <c r="D3" s="30"/>
       <c r="E3" s="13"/>
       <c r="F3" s="31"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="32"/>
@@ -2038,7 +2137,7 @@
       <c r="F4" s="31"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="32"/>
@@ -2047,7 +2146,7 @@
       <c r="F5" s="31"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="32"/>
@@ -2056,7 +2155,7 @@
       <c r="F6" s="31"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="32"/>
@@ -2065,7 +2164,7 @@
       <c r="F7" s="31"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="32"/>
@@ -2074,7 +2173,7 @@
       <c r="F8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="32"/>
@@ -2083,7 +2182,7 @@
       <c r="F9" s="31"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="32"/>
@@ -2092,7 +2191,7 @@
       <c r="F10" s="31"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="32"/>
@@ -2101,7 +2200,7 @@
       <c r="F11" s="31"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="32"/>
@@ -2110,7 +2209,7 @@
       <c r="F12" s="31"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="32"/>
@@ -2119,7 +2218,7 @@
       <c r="F13" s="31"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="32"/>
@@ -2128,7 +2227,7 @@
       <c r="F14" s="31"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="32"/>
@@ -2137,7 +2236,7 @@
       <c r="F15" s="31"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="32"/>
@@ -2146,7 +2245,7 @@
       <c r="F16" s="31"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="32"/>
@@ -2155,7 +2254,7 @@
       <c r="F17" s="31"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="32"/>
@@ -2188,9 +2287,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="45.2024291497976"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="45.6315789473684"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="40.919028340081"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="34" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="35" width="8.89068825910931"/>
   </cols>
@@ -2250,12 +2349,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="26" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="33.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="25" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="38" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2294,12 +2393,12 @@
         <v>7</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="29" t="s">
         <v>37</v>
       </c>
       <c r="E3" s="43" t="s">
@@ -2314,15 +2413,15 @@
         <v>7</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="29" t="s">
         <v>52</v>
       </c>
       <c r="F4" s="44" t="n">
@@ -2334,12 +2433,12 @@
         <v>7</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="29" t="s">
         <v>57</v>
       </c>
       <c r="E5" s="43" t="s">
@@ -2354,12 +2453,12 @@
         <v>20</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="43" t="s">
@@ -2373,30 +2472,30 @@
       <c r="A7" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
       <c r="F7" s="44"/>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="49"/>
       <c r="F8" s="30"/>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="49"/>
       <c r="F9" s="30"/>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="49"/>
       <c r="F10" s="30"/>
     </row>
@@ -2470,27 +2569,27 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="50" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="51" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="16" t="s">
         <v>30</v>
       </c>
@@ -2560,7 +2659,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C5" s="54" t="n">
         <v>8850886103133</v>

</xml_diff>

<commit_message>
BITH - KPI Update 1st April
</commit_message>
<xml_diff>
--- a/Projects/BITH/Data/Template.xlsx
+++ b/Projects/BITH/Data/Template.xlsx
@@ -538,7 +538,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="77">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -754,6 +754,12 @@
   </si>
   <si>
     <t xml:space="preserve">TH_Primary_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf Talker_Pharmaton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH_Primary_06</t>
   </si>
   <si>
     <t xml:space="preserve">Secondary_Dual_Bisolvon + Cepacol</t>
@@ -1428,13 +1434,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1693,17 +1699,17 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="45.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="45.8461538461538"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -1717,6 +1723,7 @@
         <v>30</v>
       </c>
       <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
@@ -2076,11 +2083,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="25" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="25" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="25" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="25" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="25" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="25" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="25" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="25" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1023" min="7" style="14" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.89068825910931"/>
   </cols>
@@ -2287,9 +2294,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="45.6315789473684"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="34" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="34" width="46.0607287449393"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="34" width="41.2388663967611"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="34" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="35" width="8.89068825910931"/>
   </cols>
@@ -2341,20 +2348,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="29.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="25" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="25" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="38" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2448,107 +2455,127 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="47" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="42" t="s">
         <v>72</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>73</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="48" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>64</v>
+      </c>
+      <c r="F6" s="45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="44"/>
-    </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="46" t="s">
+        <v>20</v>
+      </c>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="30"/>
-    </row>
-    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="29"/>
+      <c r="F8" s="44"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
       <c r="E9" s="49"/>
       <c r="F9" s="30"/>
     </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
       <c r="E10" s="49"/>
       <c r="F10" s="30"/>
     </row>
-    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="30"/>
     </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F12" s="30"/>
     </row>
-    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F13" s="30"/>
     </row>
-    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F14" s="30"/>
     </row>
-    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="30"/>
     </row>
-    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="30"/>
     </row>
-    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="30"/>
     </row>
-    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="30"/>
     </row>
-    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F19" s="30"/>
     </row>
-    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F20" s="30"/>
     </row>
-    <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F21" s="30"/>
     </row>
-    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F22" s="30"/>
     </row>
-    <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F23" s="30"/>
     </row>
-    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F24" s="30"/>
     </row>
-    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="30"/>
     </row>
-    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F26" s="30"/>
     </row>
-    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="30"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F28" s="30"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2567,20 +2594,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F65536"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="32.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="45.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="45.8461538461538"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="18.3157894736842"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="50" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="51" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2659,7 +2686,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C5" s="54" t="n">
         <v>8850886103133</v>
@@ -2715,20 +2742,20 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="56" t="s">
-        <v>22</v>
+      <c r="A8" s="53" t="s">
+        <v>12</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C8" s="54" t="n">
-        <v>8850886103058</v>
+        <v>8850886103171</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>38</v>
+        <v>63</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>64</v>
       </c>
       <c r="F8" s="55" t="n">
         <v>1</v>
@@ -2739,13 +2766,13 @@
         <v>22</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C9" s="54" t="n">
-        <v>8850886057252</v>
+        <v>8850886103058</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>38</v>
@@ -2754,12 +2781,66 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="54" t="n">
+        <v>8850886057252</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="54" t="n">
+        <v>8850886103171</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="54" t="n">
+        <v>4048846004130</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="55" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>